<commit_message>
Updated Cantt Chart with Deadlines
</commit_message>
<xml_diff>
--- a/Gantt_Chart.xlsx
+++ b/Gantt_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linja\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15FDB6CC-EE3F-4094-822A-43072087726F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DE9F23-5DEB-49D8-AADF-3DAAF307A999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8832" yWindow="0" windowWidth="14208" windowHeight="10716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="96">
   <si>
     <t>GANTT CHART</t>
   </si>
@@ -119,13 +119,145 @@
     <t>3.2.1</t>
   </si>
   <si>
-    <t>3.2.2</t>
-  </si>
-  <si>
-    <t>3.3.1</t>
-  </si>
-  <si>
     <t>Jacy Lin</t>
+  </si>
+  <si>
+    <t>Edu Planner (Cloud Based)</t>
+  </si>
+  <si>
+    <t>W1 9/4/2023</t>
+  </si>
+  <si>
+    <t>W2 9/11/2023</t>
+  </si>
+  <si>
+    <t>W3 9/18/2023</t>
+  </si>
+  <si>
+    <t>W4 9/25/2023</t>
+  </si>
+  <si>
+    <t>W5 10/2/2023</t>
+  </si>
+  <si>
+    <t>W6 10/9/2023</t>
+  </si>
+  <si>
+    <t>W7 10/16/2023</t>
+  </si>
+  <si>
+    <t>W8 10/23/2023</t>
+  </si>
+  <si>
+    <t>W9 10/30/2023</t>
+  </si>
+  <si>
+    <t>W10 11/06/2023</t>
+  </si>
+  <si>
+    <t>W11 11/13/2023</t>
+  </si>
+  <si>
+    <t>W12 11/20/2023</t>
+  </si>
+  <si>
+    <t>W13 11/27/2023</t>
+  </si>
+  <si>
+    <t>W14 12/4/2023</t>
+  </si>
+  <si>
+    <t>Create a Template</t>
+  </si>
+  <si>
+    <t>Create a Theme</t>
+  </si>
+  <si>
+    <t>Jacy</t>
+  </si>
+  <si>
+    <t>Data Management</t>
+  </si>
+  <si>
+    <t>4.2.1</t>
+  </si>
+  <si>
+    <t>4.2.2</t>
+  </si>
+  <si>
+    <t>4.3.1</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>Angel</t>
+  </si>
+  <si>
+    <t>Create a Sample Flowchart</t>
+  </si>
+  <si>
+    <t>File/Folder Structuring</t>
+  </si>
+  <si>
+    <t>Data Base Schema Design</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Login Page</t>
+  </si>
+  <si>
+    <t>Sign Up Page</t>
+  </si>
+  <si>
+    <t>Create an HTML/CSS Page</t>
+  </si>
+  <si>
+    <t>Ask school for Data Permission</t>
+  </si>
+  <si>
+    <t>Setting Up</t>
+  </si>
+  <si>
+    <t>First Week</t>
+  </si>
+  <si>
+    <t>Designing</t>
+  </si>
+  <si>
+    <t>Database Setup</t>
+  </si>
+  <si>
+    <t>Sign-Up Page</t>
+  </si>
+  <si>
+    <t>Calendar Page</t>
+  </si>
+  <si>
+    <t>Classes Page</t>
+  </si>
+  <si>
+    <t>Faculty List</t>
+  </si>
+  <si>
+    <t>Profile Page</t>
+  </si>
+  <si>
+    <t>HTML/CSS - Login Page</t>
+  </si>
+  <si>
+    <t>HTML/CSS - Sign Up Page</t>
+  </si>
+  <si>
+    <t>SSH Access/Web Servers</t>
+  </si>
+  <si>
+    <t>Generate Data Base (PHP)</t>
   </si>
   <si>
     <r>
@@ -162,7 +294,25 @@
         <color rgb="FF000000"/>
         <rFont val="Roboto"/>
       </rPr>
-      <t xml:space="preserve">, Ramses Terry, </t>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>Ramses Terry</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
     </r>
     <r>
       <rPr>
@@ -193,85 +343,79 @@
     </r>
   </si>
   <si>
-    <t>Edu Planner (Cloud Based)</t>
-  </si>
-  <si>
-    <t>W1 9/4/2023</t>
-  </si>
-  <si>
-    <t>W2 9/11/2023</t>
-  </si>
-  <si>
-    <t>W3 9/18/2023</t>
-  </si>
-  <si>
-    <t>W4 9/25/2023</t>
-  </si>
-  <si>
-    <t>W5 10/2/2023</t>
-  </si>
-  <si>
-    <t>W6 10/9/2023</t>
-  </si>
-  <si>
-    <t>W7 10/16/2023</t>
-  </si>
-  <si>
-    <t>W8 10/23/2023</t>
-  </si>
-  <si>
-    <t>W9 10/30/2023</t>
-  </si>
-  <si>
-    <t>W10 11/06/2023</t>
-  </si>
-  <si>
-    <t>W11 11/13/2023</t>
-  </si>
-  <si>
-    <t>W12 11/20/2023</t>
-  </si>
-  <si>
-    <t>W13 11/27/2023</t>
-  </si>
-  <si>
-    <t>W14 12/4/2023</t>
-  </si>
-  <si>
-    <t>Create a Template</t>
-  </si>
-  <si>
-    <t>Create a Theme</t>
-  </si>
-  <si>
-    <t>Jacy</t>
-  </si>
-  <si>
-    <t>Data Management</t>
-  </si>
-  <si>
-    <t>4.2.1</t>
-  </si>
-  <si>
-    <t>4.2.2</t>
-  </si>
-  <si>
-    <t>4.3.1</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Everyone</t>
-  </si>
-  <si>
-    <t>1 Week</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1 Week</t>
-  </si>
-  <si>
-    <t>Angel</t>
+    <t>Ramses</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>Jacy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>/Ramses</t>
+    </r>
+  </si>
+  <si>
+    <t>HTML/CSS - Calendar Page</t>
+  </si>
+  <si>
+    <t>HTML/CSS - Classes Page</t>
+  </si>
+  <si>
+    <t>HTML/CSS - Faculty Page</t>
+  </si>
+  <si>
+    <t>HTML/CSS - Profile Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Github - Login Page Maintanence </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Github - Sign Page Maintanence </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Github - Calendar Page Maintanence </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Github - Classes Page Maintanence </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Github - Profile Page Maintanence </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Github - Faculty Page Maintanence </t>
+  </si>
+  <si>
+    <t>Maintanence - Ensure Page Works</t>
+  </si>
+  <si>
+    <t>Design an overall flowchart</t>
+  </si>
+  <si>
+    <t>Flowchart - Login Page</t>
+  </si>
+  <si>
+    <t>Flowchart - Sign Up Page</t>
+  </si>
+  <si>
+    <t>Flowchart - Calendar Page</t>
+  </si>
+  <si>
+    <t>Flowchart - Classes Page</t>
+  </si>
+  <si>
+    <t>Flowchart - Faculty Page</t>
+  </si>
+  <si>
+    <t>Flowchart - Profile Page</t>
   </si>
 </sst>
 </file>
@@ -282,7 +426,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -464,8 +608,51 @@
       <color rgb="FFFF0000"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="9"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF7030A0"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -550,8 +737,26 @@
         <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFDDEBF7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFEDEDED"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -697,11 +902,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -848,12 +1064,6 @@
     <xf numFmtId="0" fontId="27" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="27" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -866,6 +1076,10 @@
     <xf numFmtId="0" fontId="27" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -912,6 +1126,42 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="27" fillId="15" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="15" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -929,10 +1179,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1237,10 +1483,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BZ44"/>
+  <dimension ref="A1:BZ53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="81" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AC40" sqref="AC40:AG40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1749,7 @@
       </c>
       <c r="C4" s="65"/>
       <c r="D4" s="75" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E4" s="67"/>
       <c r="F4" s="67"/>
@@ -1678,7 +1924,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -1764,7 +2010,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -1946,98 +2192,98 @@
       <c r="G9" s="70"/>
       <c r="H9" s="78"/>
       <c r="I9" s="61" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J9" s="62"/>
       <c r="K9" s="62"/>
       <c r="L9" s="62"/>
       <c r="M9" s="63"/>
       <c r="N9" s="61" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="O9" s="62"/>
       <c r="P9" s="62"/>
       <c r="Q9" s="62"/>
       <c r="R9" s="63"/>
       <c r="S9" s="61" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="T9" s="62"/>
       <c r="U9" s="62"/>
       <c r="V9" s="62"/>
       <c r="W9" s="63"/>
       <c r="X9" s="61" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="Y9" s="62"/>
       <c r="Z9" s="62"/>
       <c r="AA9" s="62"/>
       <c r="AB9" s="63"/>
       <c r="AC9" s="61" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AD9" s="62"/>
       <c r="AE9" s="62"/>
       <c r="AF9" s="62"/>
       <c r="AG9" s="63"/>
       <c r="AH9" s="61" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="AI9" s="62"/>
       <c r="AJ9" s="62"/>
       <c r="AK9" s="62"/>
       <c r="AL9" s="63"/>
       <c r="AM9" s="61" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="AN9" s="62"/>
       <c r="AO9" s="62"/>
       <c r="AP9" s="62"/>
       <c r="AQ9" s="63"/>
       <c r="AR9" s="61" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="AS9" s="62"/>
       <c r="AT9" s="62"/>
       <c r="AU9" s="62"/>
       <c r="AV9" s="63"/>
       <c r="AW9" s="61" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AX9" s="62"/>
       <c r="AY9" s="62"/>
       <c r="AZ9" s="62"/>
       <c r="BA9" s="63"/>
       <c r="BB9" s="61" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="BC9" s="62"/>
       <c r="BD9" s="62"/>
       <c r="BE9" s="62"/>
       <c r="BF9" s="63"/>
       <c r="BG9" s="61" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="BH9" s="62"/>
       <c r="BI9" s="62"/>
       <c r="BJ9" s="62"/>
       <c r="BK9" s="63"/>
       <c r="BL9" s="61" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="BM9" s="62"/>
       <c r="BN9" s="62"/>
       <c r="BO9" s="62"/>
       <c r="BP9" s="63"/>
       <c r="BQ9" s="61" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="BR9" s="62"/>
       <c r="BS9" s="62"/>
       <c r="BT9" s="62"/>
       <c r="BU9" s="63"/>
       <c r="BV9" s="61" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="BW9" s="62"/>
       <c r="BX9" s="62"/>
@@ -2059,72 +2305,100 @@
       <c r="H10" s="28"/>
       <c r="I10" s="29"/>
       <c r="J10" s="30"/>
-      <c r="K10" s="31"/>
+      <c r="K10" s="31" t="s">
+        <v>63</v>
+      </c>
       <c r="L10" s="31"/>
       <c r="M10" s="29"/>
       <c r="N10" s="29"/>
       <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
+      <c r="P10" s="29" t="s">
+        <v>62</v>
+      </c>
       <c r="Q10" s="29"/>
       <c r="R10" s="29"/>
       <c r="S10" s="29"/>
       <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
+      <c r="U10" s="29" t="s">
+        <v>64</v>
+      </c>
       <c r="V10" s="29"/>
       <c r="W10" s="29"/>
       <c r="X10" s="29"/>
       <c r="Y10" s="29"/>
-      <c r="Z10" s="29"/>
+      <c r="Z10" s="29" t="s">
+        <v>65</v>
+      </c>
       <c r="AA10" s="29"/>
       <c r="AB10" s="29"/>
       <c r="AC10" s="29"/>
       <c r="AD10" s="29"/>
-      <c r="AE10" s="29"/>
+      <c r="AE10" s="29" t="s">
+        <v>58</v>
+      </c>
       <c r="AF10" s="29"/>
       <c r="AG10" s="29"/>
       <c r="AH10" s="29"/>
       <c r="AI10" s="29"/>
-      <c r="AJ10" s="29"/>
+      <c r="AJ10" s="29" t="s">
+        <v>66</v>
+      </c>
       <c r="AK10" s="29"/>
       <c r="AL10" s="29"/>
       <c r="AM10" s="29"/>
       <c r="AN10" s="29"/>
-      <c r="AO10" s="29"/>
+      <c r="AO10" s="29" t="s">
+        <v>67</v>
+      </c>
       <c r="AP10" s="29"/>
       <c r="AQ10" s="29"/>
       <c r="AR10" s="29"/>
       <c r="AS10" s="29"/>
-      <c r="AT10" s="29"/>
+      <c r="AT10" s="29" t="s">
+        <v>67</v>
+      </c>
       <c r="AU10" s="29"/>
       <c r="AV10" s="29"/>
       <c r="AW10" s="29"/>
       <c r="AX10" s="29"/>
-      <c r="AY10" s="29"/>
+      <c r="AY10" s="29" t="s">
+        <v>68</v>
+      </c>
       <c r="AZ10" s="29"/>
       <c r="BA10" s="29"/>
       <c r="BB10" s="29"/>
       <c r="BC10" s="29"/>
-      <c r="BD10" s="29"/>
+      <c r="BD10" s="29" t="s">
+        <v>68</v>
+      </c>
       <c r="BE10" s="29"/>
       <c r="BF10" s="29"/>
       <c r="BG10" s="29"/>
       <c r="BH10" s="29"/>
-      <c r="BI10" s="29"/>
+      <c r="BI10" s="29" t="s">
+        <v>69</v>
+      </c>
       <c r="BJ10" s="29"/>
       <c r="BK10" s="29"/>
       <c r="BL10" s="29"/>
       <c r="BM10" s="29"/>
-      <c r="BN10" s="29"/>
+      <c r="BN10" s="29" t="s">
+        <v>69</v>
+      </c>
       <c r="BO10" s="29"/>
       <c r="BP10" s="29"/>
       <c r="BQ10" s="29"/>
       <c r="BR10" s="29"/>
-      <c r="BS10" s="29"/>
+      <c r="BS10" s="29" t="s">
+        <v>70</v>
+      </c>
       <c r="BT10" s="29"/>
       <c r="BU10" s="29"/>
       <c r="BV10" s="29"/>
       <c r="BW10" s="29"/>
-      <c r="BX10" s="29"/>
+      <c r="BX10" s="29" t="s">
+        <v>70</v>
+      </c>
       <c r="BY10" s="29"/>
       <c r="BZ10" s="29"/>
     </row>
@@ -2136,21 +2410,25 @@
       <c r="C11" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
+      <c r="D11" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="35">
+        <v>45166</v>
+      </c>
+      <c r="F11" s="35">
+        <v>45173</v>
+      </c>
       <c r="G11" s="36">
         <f t="shared" ref="G11:G17" si="0">DAYS360(E11,F11)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H11" s="37"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
       <c r="N11" s="42"/>
       <c r="O11" s="42"/>
       <c r="P11" s="42"/>
@@ -2225,21 +2503,25 @@
       <c r="C12" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
+      <c r="D12" s="86" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="35">
+        <v>45166</v>
+      </c>
+      <c r="F12" s="35">
+        <v>45173</v>
+      </c>
       <c r="G12" s="36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H12" s="37"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="55"/>
+      <c r="M12" s="55"/>
       <c r="N12" s="42"/>
       <c r="O12" s="42"/>
       <c r="P12" s="42"/>
@@ -2315,20 +2597,24 @@
         <v>21</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
+        <v>52</v>
+      </c>
+      <c r="E13" s="35">
+        <v>45166</v>
+      </c>
+      <c r="F13" s="35">
+        <v>45173</v>
+      </c>
       <c r="G13" s="36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H13" s="37"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="55"/>
+      <c r="M13" s="55"/>
       <c r="N13" s="42"/>
       <c r="O13" s="42"/>
       <c r="P13" s="42"/>
@@ -2403,21 +2689,25 @@
       <c r="C14" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
+      <c r="D14" s="86" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="35">
+        <v>45173</v>
+      </c>
+      <c r="F14" s="35">
+        <v>45175</v>
+      </c>
       <c r="G14" s="36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H14" s="37"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="56"/>
       <c r="N14" s="42"/>
       <c r="O14" s="42"/>
       <c r="P14" s="42"/>
@@ -2493,20 +2783,24 @@
         <v>23</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
+        <v>52</v>
+      </c>
+      <c r="E15" s="35">
+        <v>45166</v>
+      </c>
+      <c r="F15" s="35">
+        <v>45173</v>
+      </c>
       <c r="G15" s="36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H15" s="37"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="56"/>
       <c r="N15" s="42"/>
       <c r="O15" s="42"/>
       <c r="P15" s="42"/>
@@ -2578,25 +2872,33 @@
       <c r="B16" s="33">
         <v>1.5</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
+      <c r="C16" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="86" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="35">
+        <v>45182</v>
+      </c>
+      <c r="F16" s="35">
+        <v>45189</v>
+      </c>
       <c r="G16" s="36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H16" s="37"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
+      <c r="I16" s="83"/>
+      <c r="J16" s="83"/>
+      <c r="K16" s="83"/>
+      <c r="L16" s="83"/>
+      <c r="M16" s="83"/>
+      <c r="N16" s="84"/>
+      <c r="O16" s="84"/>
+      <c r="P16" s="84"/>
+      <c r="Q16" s="84"/>
+      <c r="R16" s="84"/>
       <c r="S16" s="38"/>
       <c r="T16" s="38"/>
       <c r="U16" s="38"/>
@@ -2661,27 +2963,35 @@
     <row r="17" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="32"/>
       <c r="B17" s="33">
-        <v>1.6</v>
-      </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
+        <v>1.5</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="87" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="35">
+        <v>45182</v>
+      </c>
+      <c r="F17" s="35">
+        <v>45189</v>
+      </c>
       <c r="G17" s="36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H17" s="37"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="42"/>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="82"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="82"/>
+      <c r="N17" s="84"/>
+      <c r="O17" s="84"/>
+      <c r="P17" s="84"/>
+      <c r="Q17" s="84"/>
+      <c r="R17" s="84"/>
       <c r="S17" s="38"/>
       <c r="T17" s="38"/>
       <c r="U17" s="38"/>
@@ -2756,11 +3066,11 @@
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
       <c r="H18" s="28"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="54"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="52"/>
       <c r="N18" s="29"/>
       <c r="O18" s="29"/>
       <c r="P18" s="29"/>
@@ -2833,10 +3143,10 @@
         <v>2.1</v>
       </c>
       <c r="C19" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>49</v>
+        <v>44</v>
+      </c>
+      <c r="D19" s="86" t="s">
+        <v>46</v>
       </c>
       <c r="E19" s="35">
         <v>45180</v>
@@ -2844,20 +3154,20 @@
       <c r="F19" s="35">
         <v>45187</v>
       </c>
-      <c r="G19" s="36" t="s">
-        <v>57</v>
+      <c r="G19" s="36">
+        <v>7</v>
       </c>
       <c r="H19" s="45"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="42"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="82"/>
+      <c r="L19" s="82"/>
+      <c r="M19" s="82"/>
+      <c r="N19" s="84"/>
+      <c r="O19" s="84"/>
+      <c r="P19" s="84"/>
+      <c r="Q19" s="84"/>
+      <c r="R19" s="84"/>
       <c r="S19" s="38"/>
       <c r="T19" s="38"/>
       <c r="U19" s="38"/>
@@ -2925,10 +3235,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C20" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="34" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="D20" s="86" t="s">
+        <v>46</v>
       </c>
       <c r="E20" s="35">
         <v>45187</v>
@@ -2936,25 +3246,25 @@
       <c r="F20" s="35">
         <v>45194</v>
       </c>
-      <c r="G20" s="36" t="s">
-        <v>56</v>
+      <c r="G20" s="36">
+        <v>7</v>
       </c>
       <c r="H20" s="45"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="51"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="82"/>
+      <c r="L20" s="82"/>
+      <c r="M20" s="82"/>
       <c r="N20" s="42"/>
       <c r="O20" s="42"/>
       <c r="P20" s="42"/>
       <c r="Q20" s="42"/>
       <c r="R20" s="42"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="38"/>
-      <c r="U20" s="38"/>
-      <c r="V20" s="38"/>
-      <c r="W20" s="38"/>
+      <c r="S20" s="51"/>
+      <c r="T20" s="51"/>
+      <c r="U20" s="51"/>
+      <c r="V20" s="51"/>
+      <c r="W20" s="51"/>
       <c r="X20" s="38"/>
       <c r="Y20" s="38"/>
       <c r="Z20" s="38"/>
@@ -3016,30 +3326,37 @@
       <c r="B21" s="33">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C21" s="45"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
+      <c r="C21" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="86" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="35">
+        <v>45187</v>
+      </c>
+      <c r="F21" s="35">
+        <v>45194</v>
+      </c>
       <c r="G21" s="36">
-        <f t="shared" ref="G21" si="1">DAYS360(E21,F21)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H21" s="45"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="51"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="82"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="82"/>
       <c r="N21" s="42"/>
       <c r="O21" s="42"/>
       <c r="P21" s="42"/>
       <c r="Q21" s="42"/>
       <c r="R21" s="42"/>
-      <c r="S21" s="38"/>
-      <c r="T21" s="38"/>
-      <c r="U21" s="38"/>
-      <c r="V21" s="38"/>
-      <c r="W21" s="38"/>
+      <c r="S21" s="55"/>
+      <c r="T21" s="55"/>
+      <c r="U21" s="55"/>
+      <c r="V21" s="55"/>
+      <c r="W21" s="55"/>
       <c r="X21" s="38"/>
       <c r="Y21" s="38"/>
       <c r="Z21" s="38"/>
@@ -3101,24 +3418,32 @@
       <c r="B22" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="45"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
+      <c r="C22" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="88" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="35">
+        <v>45180</v>
+      </c>
+      <c r="F22" s="35">
+        <v>45187</v>
+      </c>
       <c r="G22" s="36">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H22" s="45"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="51"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="42"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="81"/>
+      <c r="K22" s="82"/>
+      <c r="L22" s="82"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="84"/>
+      <c r="O22" s="84"/>
+      <c r="P22" s="84"/>
+      <c r="Q22" s="84"/>
+      <c r="R22" s="84"/>
       <c r="S22" s="38"/>
       <c r="T22" s="38"/>
       <c r="U22" s="38"/>
@@ -3185,30 +3510,38 @@
       <c r="B23" s="33">
         <v>2.4</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
+      <c r="C23" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="35">
+        <v>45182</v>
+      </c>
+      <c r="F23" s="35">
+        <v>45189</v>
+      </c>
       <c r="G23" s="36">
-        <f t="shared" ref="G23:G24" si="2">DAYS360(E23,F23)</f>
-        <v>0</v>
+        <f t="shared" ref="G23" si="1">DAYS360(E23,F23)</f>
+        <v>7</v>
       </c>
       <c r="H23" s="45"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
+      <c r="I23" s="80"/>
+      <c r="J23" s="81"/>
+      <c r="K23" s="82"/>
+      <c r="L23" s="82"/>
+      <c r="M23" s="82"/>
       <c r="N23" s="42"/>
       <c r="O23" s="42"/>
       <c r="P23" s="42"/>
       <c r="Q23" s="42"/>
       <c r="R23" s="42"/>
-      <c r="S23" s="38"/>
-      <c r="T23" s="38"/>
-      <c r="U23" s="38"/>
-      <c r="V23" s="38"/>
-      <c r="W23" s="38"/>
+      <c r="S23" s="55"/>
+      <c r="T23" s="55"/>
+      <c r="U23" s="55"/>
+      <c r="V23" s="55"/>
+      <c r="W23" s="55"/>
       <c r="X23" s="38"/>
       <c r="Y23" s="38"/>
       <c r="Z23" s="38"/>
@@ -3270,20 +3603,27 @@
       <c r="B24" s="33">
         <v>2.5</v>
       </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
+      <c r="C24" s="57" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="35">
+        <v>45189</v>
+      </c>
+      <c r="F24" s="35">
+        <v>45196</v>
+      </c>
       <c r="G24" s="36">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H24" s="45"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="51"/>
-      <c r="M24" s="51"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="81"/>
+      <c r="K24" s="82"/>
+      <c r="L24" s="82"/>
+      <c r="M24" s="82"/>
       <c r="N24" s="42"/>
       <c r="O24" s="42"/>
       <c r="P24" s="42"/>
@@ -3294,11 +3634,11 @@
       <c r="U24" s="38"/>
       <c r="V24" s="38"/>
       <c r="W24" s="38"/>
-      <c r="X24" s="38"/>
-      <c r="Y24" s="38"/>
-      <c r="Z24" s="38"/>
-      <c r="AA24" s="38"/>
-      <c r="AB24" s="38"/>
+      <c r="X24" s="55"/>
+      <c r="Y24" s="55"/>
+      <c r="Z24" s="55"/>
+      <c r="AA24" s="55"/>
+      <c r="AB24" s="55"/>
       <c r="AC24" s="39"/>
       <c r="AD24" s="39"/>
       <c r="AE24" s="39"/>
@@ -3355,19 +3695,27 @@
       <c r="B25" s="33">
         <v>2.6</v>
       </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
+      <c r="C25" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="35">
+        <v>45203</v>
+      </c>
+      <c r="F25" s="35">
+        <v>45210</v>
+      </c>
       <c r="G25" s="36">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H25" s="45"/>
-      <c r="I25" s="52"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="51"/>
-      <c r="M25" s="51"/>
+      <c r="I25" s="80"/>
+      <c r="J25" s="81"/>
+      <c r="K25" s="82"/>
+      <c r="L25" s="82"/>
+      <c r="M25" s="82"/>
       <c r="N25" s="42"/>
       <c r="O25" s="42"/>
       <c r="P25" s="42"/>
@@ -3439,20 +3787,28 @@
       <c r="B26" s="33">
         <v>2.7</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
+      <c r="C26" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="35">
+        <v>45210</v>
+      </c>
+      <c r="F26" s="35">
+        <v>45217</v>
+      </c>
       <c r="G26" s="36">
-        <f t="shared" ref="G26:G27" si="3">DAYS360(E26,F26)</f>
-        <v>0</v>
+        <f t="shared" ref="G26:G27" si="2">DAYS360(E26,F26)</f>
+        <v>7</v>
       </c>
       <c r="H26" s="45"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="51"/>
-      <c r="L26" s="51"/>
-      <c r="M26" s="51"/>
+      <c r="I26" s="80"/>
+      <c r="J26" s="81"/>
+      <c r="K26" s="82"/>
+      <c r="L26" s="82"/>
+      <c r="M26" s="82"/>
       <c r="N26" s="42"/>
       <c r="O26" s="42"/>
       <c r="P26" s="42"/>
@@ -3524,20 +3880,27 @@
       <c r="B27" s="33">
         <v>2.8</v>
       </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
+      <c r="C27" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="35">
+        <v>45217</v>
+      </c>
+      <c r="F27" s="35">
+        <v>45231</v>
+      </c>
       <c r="G27" s="36">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H27" s="45"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="51"/>
-      <c r="M27" s="51"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="81"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="82"/>
       <c r="N27" s="42"/>
       <c r="O27" s="42"/>
       <c r="P27" s="42"/>
@@ -3609,19 +3972,27 @@
       <c r="B28" s="33">
         <v>2.9</v>
       </c>
-      <c r="C28" s="45"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
+      <c r="C28" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="35">
+        <v>45231</v>
+      </c>
+      <c r="F28" s="35">
+        <v>45245</v>
+      </c>
       <c r="G28" s="36">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H28" s="45"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="53"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="51"/>
+      <c r="I28" s="80"/>
+      <c r="J28" s="81"/>
+      <c r="K28" s="82"/>
+      <c r="L28" s="82"/>
+      <c r="M28" s="82"/>
       <c r="N28" s="42"/>
       <c r="O28" s="42"/>
       <c r="P28" s="42"/>
@@ -3693,20 +4064,28 @@
       <c r="B29" s="44">
         <v>2.1</v>
       </c>
-      <c r="C29" s="45"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
+      <c r="C29" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="35">
+        <v>45245</v>
+      </c>
+      <c r="F29" s="35">
+        <v>45259</v>
+      </c>
       <c r="G29" s="36">
         <f>DAYS360(E29,F29)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H29" s="45"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="51"/>
-      <c r="L29" s="51"/>
-      <c r="M29" s="51"/>
+      <c r="I29" s="80"/>
+      <c r="J29" s="81"/>
+      <c r="K29" s="82"/>
+      <c r="L29" s="82"/>
+      <c r="M29" s="82"/>
       <c r="N29" s="42"/>
       <c r="O29" s="42"/>
       <c r="P29" s="42"/>
@@ -3778,19 +4157,27 @@
       <c r="B30" s="44">
         <v>2.11</v>
       </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
+      <c r="C30" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" s="35">
+        <v>45259</v>
+      </c>
+      <c r="F30" s="35">
+        <v>45273</v>
+      </c>
       <c r="G30" s="36">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H30" s="45"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="51"/>
-      <c r="L30" s="51"/>
-      <c r="M30" s="51"/>
+      <c r="I30" s="80"/>
+      <c r="J30" s="81"/>
+      <c r="K30" s="82"/>
+      <c r="L30" s="82"/>
+      <c r="M30" s="82"/>
       <c r="N30" s="42"/>
       <c r="O30" s="42"/>
       <c r="P30" s="42"/>
@@ -3870,11 +4257,11 @@
       <c r="F31" s="28"/>
       <c r="G31" s="28"/>
       <c r="H31" s="28"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="55"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="56"/>
-      <c r="M31" s="54"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="54"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="52"/>
       <c r="N31" s="29"/>
       <c r="O31" s="29"/>
       <c r="P31" s="29"/>
@@ -3946,20 +4333,28 @@
       <c r="B32" s="33">
         <v>3.1</v>
       </c>
-      <c r="C32" s="45"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
+      <c r="C32" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="88" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="35">
+        <v>45189</v>
+      </c>
+      <c r="F32" s="35">
+        <v>45196</v>
+      </c>
       <c r="G32" s="36">
         <f>DAYS360(E32,F32)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H32" s="37"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="51"/>
-      <c r="L32" s="51"/>
-      <c r="M32" s="51"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="81"/>
+      <c r="K32" s="82"/>
+      <c r="L32" s="82"/>
+      <c r="M32" s="82"/>
       <c r="N32" s="42"/>
       <c r="O32" s="42"/>
       <c r="P32" s="42"/>
@@ -3970,11 +4365,11 @@
       <c r="U32" s="38"/>
       <c r="V32" s="38"/>
       <c r="W32" s="38"/>
-      <c r="X32" s="38"/>
-      <c r="Y32" s="38"/>
-      <c r="Z32" s="38"/>
-      <c r="AA32" s="38"/>
-      <c r="AB32" s="38"/>
+      <c r="X32" s="55"/>
+      <c r="Y32" s="55"/>
+      <c r="Z32" s="55"/>
+      <c r="AA32" s="55"/>
+      <c r="AB32" s="55"/>
       <c r="AC32" s="39"/>
       <c r="AD32" s="39"/>
       <c r="AE32" s="39"/>
@@ -4031,19 +4426,27 @@
       <c r="B33" s="33">
         <v>3.2</v>
       </c>
-      <c r="C33" s="45"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
+      <c r="C33" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="88" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" s="35">
+        <v>45203</v>
+      </c>
+      <c r="F33" s="35">
+        <v>45210</v>
+      </c>
       <c r="G33" s="36">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H33" s="37"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="51"/>
-      <c r="L33" s="51"/>
-      <c r="M33" s="51"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="81"/>
+      <c r="K33" s="82"/>
+      <c r="L33" s="82"/>
+      <c r="M33" s="82"/>
       <c r="N33" s="42"/>
       <c r="O33" s="42"/>
       <c r="P33" s="42"/>
@@ -4059,11 +4462,11 @@
       <c r="Z33" s="38"/>
       <c r="AA33" s="38"/>
       <c r="AB33" s="38"/>
-      <c r="AC33" s="39"/>
-      <c r="AD33" s="39"/>
-      <c r="AE33" s="39"/>
-      <c r="AF33" s="39"/>
-      <c r="AG33" s="39"/>
+      <c r="AC33" s="91"/>
+      <c r="AD33" s="91"/>
+      <c r="AE33" s="91"/>
+      <c r="AF33" s="91"/>
+      <c r="AG33" s="91"/>
       <c r="AH33" s="38"/>
       <c r="AI33" s="38"/>
       <c r="AJ33" s="38"/>
@@ -4115,20 +4518,28 @@
       <c r="B34" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="45"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
+      <c r="C34" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="88" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="35">
+        <v>45210</v>
+      </c>
+      <c r="F34" s="35">
+        <v>45217</v>
+      </c>
       <c r="G34" s="36">
-        <f t="shared" ref="G34:G36" si="4">DAYS360(E34,F34)</f>
-        <v>0</v>
+        <f t="shared" ref="G34:G36" si="3">DAYS360(E34,F34)</f>
+        <v>7</v>
       </c>
       <c r="H34" s="37"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="51"/>
-      <c r="L34" s="51"/>
-      <c r="M34" s="51"/>
+      <c r="I34" s="80"/>
+      <c r="J34" s="81"/>
+      <c r="K34" s="82"/>
+      <c r="L34" s="82"/>
+      <c r="M34" s="82"/>
       <c r="N34" s="42"/>
       <c r="O34" s="42"/>
       <c r="P34" s="42"/>
@@ -4197,22 +4608,29 @@
     </row>
     <row r="35" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="32"/>
-      <c r="B35" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="45"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
+      <c r="B35" s="33">
+        <v>3.3</v>
+      </c>
+      <c r="C35" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="88" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" s="35">
+        <v>45217</v>
+      </c>
+      <c r="F35" s="35">
+        <v>45231</v>
+      </c>
       <c r="G35" s="36">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I35" s="52"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="51"/>
-      <c r="L35" s="51"/>
-      <c r="M35" s="51"/>
+        <v>14</v>
+      </c>
+      <c r="I35" s="80"/>
+      <c r="J35" s="81"/>
+      <c r="K35" s="82"/>
+      <c r="L35" s="82"/>
+      <c r="M35" s="82"/>
       <c r="N35" s="42"/>
       <c r="O35" s="42"/>
       <c r="P35" s="42"/>
@@ -4282,22 +4700,30 @@
     <row r="36" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="32"/>
       <c r="B36" s="33">
-        <v>3.3</v>
-      </c>
-      <c r="C36" s="45"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
+        <v>3.5</v>
+      </c>
+      <c r="C36" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36" s="88" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="35">
+        <v>45231</v>
+      </c>
+      <c r="F36" s="35">
+        <v>45245</v>
+      </c>
       <c r="G36" s="36">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>14</v>
       </c>
       <c r="H36" s="37"/>
-      <c r="I36" s="52"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="51"/>
-      <c r="L36" s="51"/>
-      <c r="M36" s="51"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="81"/>
+      <c r="K36" s="82"/>
+      <c r="L36" s="82"/>
+      <c r="M36" s="82"/>
       <c r="N36" s="42"/>
       <c r="O36" s="42"/>
       <c r="P36" s="42"/>
@@ -4366,22 +4792,30 @@
     </row>
     <row r="37" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="32"/>
-      <c r="B37" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" s="45"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
+      <c r="B37" s="33">
+        <v>3.6</v>
+      </c>
+      <c r="C37" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="88" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" s="35">
+        <v>45245</v>
+      </c>
+      <c r="F37" s="35">
+        <v>45259</v>
+      </c>
       <c r="G37" s="36">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H37" s="37"/>
-      <c r="I37" s="52"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="51"/>
-      <c r="L37" s="51"/>
-      <c r="M37" s="51"/>
+      <c r="I37" s="80"/>
+      <c r="J37" s="81"/>
+      <c r="K37" s="82"/>
+      <c r="L37" s="82"/>
+      <c r="M37" s="82"/>
       <c r="N37" s="42"/>
       <c r="O37" s="42"/>
       <c r="P37" s="42"/>
@@ -4448,197 +4882,209 @@
       <c r="BY37" s="38"/>
       <c r="BZ37" s="38"/>
     </row>
-    <row r="38" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="B38" s="26">
+    <row r="38" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="32"/>
+      <c r="B38" s="33">
+        <v>3.7</v>
+      </c>
+      <c r="C38" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="88" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="35">
+        <v>45259</v>
+      </c>
+      <c r="F38" s="35">
+        <v>45273</v>
+      </c>
+      <c r="G38" s="36">
+        <v>14</v>
+      </c>
+      <c r="H38" s="37"/>
+      <c r="I38" s="80"/>
+      <c r="J38" s="81"/>
+      <c r="K38" s="82"/>
+      <c r="L38" s="82"/>
+      <c r="M38" s="82"/>
+      <c r="N38" s="42"/>
+      <c r="O38" s="42"/>
+      <c r="P38" s="42"/>
+      <c r="Q38" s="42"/>
+      <c r="R38" s="42"/>
+      <c r="S38" s="38"/>
+      <c r="T38" s="38"/>
+      <c r="U38" s="38"/>
+      <c r="V38" s="38"/>
+      <c r="W38" s="38"/>
+      <c r="X38" s="38"/>
+      <c r="Y38" s="38"/>
+      <c r="Z38" s="38"/>
+      <c r="AA38" s="38"/>
+      <c r="AB38" s="38"/>
+      <c r="AC38" s="39"/>
+      <c r="AD38" s="39"/>
+      <c r="AE38" s="39"/>
+      <c r="AF38" s="39"/>
+      <c r="AG38" s="39"/>
+      <c r="AH38" s="38"/>
+      <c r="AI38" s="38"/>
+      <c r="AJ38" s="38"/>
+      <c r="AK38" s="38"/>
+      <c r="AL38" s="38"/>
+      <c r="AM38" s="38"/>
+      <c r="AN38" s="38"/>
+      <c r="AO38" s="38"/>
+      <c r="AP38" s="38"/>
+      <c r="AQ38" s="38"/>
+      <c r="AR38" s="40"/>
+      <c r="AS38" s="40"/>
+      <c r="AT38" s="40"/>
+      <c r="AU38" s="40"/>
+      <c r="AV38" s="40"/>
+      <c r="AW38" s="38"/>
+      <c r="AX38" s="38"/>
+      <c r="AY38" s="38"/>
+      <c r="AZ38" s="38"/>
+      <c r="BA38" s="38"/>
+      <c r="BB38" s="38"/>
+      <c r="BC38" s="38"/>
+      <c r="BD38" s="38"/>
+      <c r="BE38" s="38"/>
+      <c r="BF38" s="38"/>
+      <c r="BG38" s="41"/>
+      <c r="BH38" s="41"/>
+      <c r="BI38" s="41"/>
+      <c r="BJ38" s="41"/>
+      <c r="BK38" s="41"/>
+      <c r="BL38" s="38"/>
+      <c r="BM38" s="38"/>
+      <c r="BN38" s="38"/>
+      <c r="BO38" s="38"/>
+      <c r="BP38" s="38"/>
+      <c r="BQ38" s="38"/>
+      <c r="BR38" s="38"/>
+      <c r="BS38" s="38"/>
+      <c r="BT38" s="38"/>
+      <c r="BU38" s="38"/>
+      <c r="BV38" s="38"/>
+      <c r="BW38" s="38"/>
+      <c r="BX38" s="38"/>
+      <c r="BY38" s="38"/>
+      <c r="BZ38" s="38"/>
+    </row>
+    <row r="39" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="26">
         <v>4</v>
       </c>
-      <c r="C38" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="54"/>
-      <c r="J38" s="55"/>
-      <c r="K38" s="56"/>
-      <c r="L38" s="56"/>
-      <c r="M38" s="54"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="29"/>
-      <c r="P38" s="29"/>
-      <c r="Q38" s="29"/>
-      <c r="R38" s="29"/>
-      <c r="S38" s="29"/>
-      <c r="T38" s="29"/>
-      <c r="U38" s="29"/>
-      <c r="V38" s="29"/>
-      <c r="W38" s="29"/>
-      <c r="X38" s="29"/>
-      <c r="Y38" s="29"/>
-      <c r="Z38" s="29"/>
-      <c r="AA38" s="29"/>
-      <c r="AB38" s="29"/>
-      <c r="AC38" s="29"/>
-      <c r="AD38" s="29"/>
-      <c r="AE38" s="29"/>
-      <c r="AF38" s="29"/>
-      <c r="AG38" s="29"/>
-      <c r="AH38" s="29"/>
-      <c r="AI38" s="29"/>
-      <c r="AJ38" s="29"/>
-      <c r="AK38" s="29"/>
-      <c r="AL38" s="29"/>
-      <c r="AM38" s="29"/>
-      <c r="AN38" s="29"/>
-      <c r="AO38" s="29"/>
-      <c r="AP38" s="29"/>
-      <c r="AQ38" s="29"/>
-      <c r="AR38" s="29"/>
-      <c r="AS38" s="29"/>
-      <c r="AT38" s="29"/>
-      <c r="AU38" s="29"/>
-      <c r="AV38" s="29"/>
-      <c r="AW38" s="29"/>
-      <c r="AX38" s="29"/>
-      <c r="AY38" s="29"/>
-      <c r="AZ38" s="29"/>
-      <c r="BA38" s="29"/>
-      <c r="BB38" s="29"/>
-      <c r="BC38" s="29"/>
-      <c r="BD38" s="29"/>
-      <c r="BE38" s="29"/>
-      <c r="BF38" s="29"/>
-      <c r="BG38" s="29"/>
-      <c r="BH38" s="29"/>
-      <c r="BI38" s="29"/>
-      <c r="BJ38" s="29"/>
-      <c r="BK38" s="29"/>
-      <c r="BL38" s="29"/>
-      <c r="BM38" s="29"/>
-      <c r="BN38" s="29"/>
-      <c r="BO38" s="29"/>
-      <c r="BP38" s="29"/>
-      <c r="BQ38" s="29"/>
-      <c r="BR38" s="29"/>
-      <c r="BS38" s="29"/>
-      <c r="BT38" s="29"/>
-      <c r="BU38" s="29"/>
-      <c r="BV38" s="29"/>
-      <c r="BW38" s="29"/>
-      <c r="BX38" s="29"/>
-      <c r="BY38" s="29"/>
-      <c r="BZ38" s="29"/>
-    </row>
-    <row r="39" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="32"/>
-      <c r="B39" s="33">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C39" s="45"/>
-      <c r="D39" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="36">
-        <f>DAYS360(E39,F39)</f>
-        <v>0</v>
-      </c>
-      <c r="H39" s="37"/>
+      <c r="C39" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
       <c r="I39" s="52"/>
       <c r="J39" s="53"/>
-      <c r="K39" s="51"/>
-      <c r="L39" s="51"/>
-      <c r="M39" s="51"/>
-      <c r="N39" s="42"/>
-      <c r="O39" s="42"/>
-      <c r="P39" s="42"/>
-      <c r="Q39" s="42"/>
-      <c r="R39" s="42"/>
-      <c r="S39" s="38"/>
-      <c r="T39" s="38"/>
-      <c r="U39" s="38"/>
-      <c r="V39" s="38"/>
-      <c r="W39" s="38"/>
-      <c r="X39" s="38"/>
-      <c r="Y39" s="38"/>
-      <c r="Z39" s="38"/>
-      <c r="AA39" s="38"/>
-      <c r="AB39" s="38"/>
-      <c r="AC39" s="39"/>
-      <c r="AD39" s="39"/>
-      <c r="AE39" s="39"/>
-      <c r="AF39" s="39"/>
-      <c r="AG39" s="39"/>
-      <c r="AH39" s="38"/>
-      <c r="AI39" s="38"/>
-      <c r="AJ39" s="38"/>
-      <c r="AK39" s="38"/>
-      <c r="AL39" s="38"/>
-      <c r="AM39" s="38"/>
-      <c r="AN39" s="38"/>
-      <c r="AO39" s="38"/>
-      <c r="AP39" s="38"/>
-      <c r="AQ39" s="38"/>
-      <c r="AR39" s="40"/>
-      <c r="AS39" s="40"/>
-      <c r="AT39" s="40"/>
-      <c r="AU39" s="40"/>
-      <c r="AV39" s="40"/>
-      <c r="AW39" s="38"/>
-      <c r="AX39" s="38"/>
-      <c r="AY39" s="38"/>
-      <c r="AZ39" s="38"/>
-      <c r="BA39" s="38"/>
-      <c r="BB39" s="38"/>
-      <c r="BC39" s="38"/>
-      <c r="BD39" s="38"/>
-      <c r="BE39" s="38"/>
-      <c r="BF39" s="38"/>
-      <c r="BG39" s="41"/>
-      <c r="BH39" s="41"/>
-      <c r="BI39" s="41"/>
-      <c r="BJ39" s="41"/>
-      <c r="BK39" s="41"/>
-      <c r="BL39" s="38"/>
-      <c r="BM39" s="38"/>
-      <c r="BN39" s="38"/>
-      <c r="BO39" s="38"/>
-      <c r="BP39" s="38"/>
-      <c r="BQ39" s="38"/>
-      <c r="BR39" s="38"/>
-      <c r="BS39" s="38"/>
-      <c r="BT39" s="38"/>
-      <c r="BU39" s="38"/>
-      <c r="BV39" s="38"/>
-      <c r="BW39" s="38"/>
-      <c r="BX39" s="38"/>
-      <c r="BY39" s="38"/>
-      <c r="BZ39" s="38"/>
+      <c r="K39" s="54"/>
+      <c r="L39" s="54"/>
+      <c r="M39" s="52"/>
+      <c r="N39" s="29"/>
+      <c r="O39" s="29"/>
+      <c r="P39" s="29"/>
+      <c r="Q39" s="29"/>
+      <c r="R39" s="29"/>
+      <c r="S39" s="29"/>
+      <c r="T39" s="29"/>
+      <c r="U39" s="29"/>
+      <c r="V39" s="29"/>
+      <c r="W39" s="29"/>
+      <c r="X39" s="29"/>
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="29"/>
+      <c r="AB39" s="29"/>
+      <c r="AC39" s="29"/>
+      <c r="AD39" s="29"/>
+      <c r="AE39" s="29"/>
+      <c r="AF39" s="29"/>
+      <c r="AG39" s="29"/>
+      <c r="AH39" s="29"/>
+      <c r="AI39" s="29"/>
+      <c r="AJ39" s="29"/>
+      <c r="AK39" s="29"/>
+      <c r="AL39" s="29"/>
+      <c r="AM39" s="29"/>
+      <c r="AN39" s="29"/>
+      <c r="AO39" s="29"/>
+      <c r="AP39" s="29"/>
+      <c r="AQ39" s="29"/>
+      <c r="AR39" s="29"/>
+      <c r="AS39" s="29"/>
+      <c r="AT39" s="29"/>
+      <c r="AU39" s="29"/>
+      <c r="AV39" s="29"/>
+      <c r="AW39" s="29"/>
+      <c r="AX39" s="29"/>
+      <c r="AY39" s="29"/>
+      <c r="AZ39" s="29"/>
+      <c r="BA39" s="29"/>
+      <c r="BB39" s="29"/>
+      <c r="BC39" s="29"/>
+      <c r="BD39" s="29"/>
+      <c r="BE39" s="29"/>
+      <c r="BF39" s="29"/>
+      <c r="BG39" s="29"/>
+      <c r="BH39" s="29"/>
+      <c r="BI39" s="29"/>
+      <c r="BJ39" s="29"/>
+      <c r="BK39" s="29"/>
+      <c r="BL39" s="29"/>
+      <c r="BM39" s="29"/>
+      <c r="BN39" s="29"/>
+      <c r="BO39" s="29"/>
+      <c r="BP39" s="29"/>
+      <c r="BQ39" s="29"/>
+      <c r="BR39" s="29"/>
+      <c r="BS39" s="29"/>
+      <c r="BT39" s="29"/>
+      <c r="BU39" s="29"/>
+      <c r="BV39" s="29"/>
+      <c r="BW39" s="29"/>
+      <c r="BX39" s="29"/>
+      <c r="BY39" s="29"/>
+      <c r="BZ39" s="29"/>
     </row>
     <row r="40" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="32"/>
       <c r="B40" s="33">
-        <v>4.2</v>
-      </c>
-      <c r="C40" s="45"/>
-      <c r="D40" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C40" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="89" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="35">
+        <v>45196</v>
+      </c>
+      <c r="F40" s="35">
+        <v>45203</v>
+      </c>
       <c r="G40" s="36">
-        <v>0</v>
+        <f>DAYS360(E40,F40)</f>
+        <v>7</v>
       </c>
       <c r="H40" s="37"/>
-      <c r="I40" s="52"/>
-      <c r="J40" s="53"/>
-      <c r="K40" s="51"/>
-      <c r="L40" s="51"/>
-      <c r="M40" s="51"/>
+      <c r="I40" s="80"/>
+      <c r="J40" s="81"/>
+      <c r="K40" s="82"/>
+      <c r="L40" s="82"/>
+      <c r="M40" s="82"/>
       <c r="N40" s="42"/>
       <c r="O40" s="42"/>
       <c r="P40" s="42"/>
@@ -4654,11 +5100,11 @@
       <c r="Z40" s="38"/>
       <c r="AA40" s="38"/>
       <c r="AB40" s="38"/>
-      <c r="AC40" s="39"/>
-      <c r="AD40" s="39"/>
-      <c r="AE40" s="39"/>
-      <c r="AF40" s="39"/>
-      <c r="AG40" s="39"/>
+      <c r="AC40" s="91"/>
+      <c r="AD40" s="91"/>
+      <c r="AE40" s="91"/>
+      <c r="AF40" s="91"/>
+      <c r="AG40" s="91"/>
       <c r="AH40" s="38"/>
       <c r="AI40" s="38"/>
       <c r="AJ40" s="38"/>
@@ -4707,25 +5153,30 @@
     </row>
     <row r="41" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="32"/>
-      <c r="B41" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" s="45"/>
-      <c r="D41" s="34" t="s">
+      <c r="B41" s="33">
+        <v>4.2</v>
+      </c>
+      <c r="C41" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
+      <c r="D41" s="89" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="35">
+        <v>45203</v>
+      </c>
+      <c r="F41" s="35">
+        <v>45210</v>
+      </c>
       <c r="G41" s="36">
-        <f t="shared" ref="G41:G43" si="5">DAYS360(E41,F41)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H41" s="37"/>
-      <c r="I41" s="52"/>
-      <c r="J41" s="53"/>
-      <c r="K41" s="51"/>
-      <c r="L41" s="51"/>
-      <c r="M41" s="51"/>
+      <c r="I41" s="80"/>
+      <c r="J41" s="81"/>
+      <c r="K41" s="82"/>
+      <c r="L41" s="82"/>
+      <c r="M41" s="82"/>
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
       <c r="P41" s="42"/>
@@ -4795,21 +5246,30 @@
     <row r="42" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="32"/>
       <c r="B42" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" s="45"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="35"/>
+        <v>48</v>
+      </c>
+      <c r="C42" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="89" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" s="35">
+        <v>45210</v>
+      </c>
+      <c r="F42" s="35">
+        <v>45217</v>
+      </c>
       <c r="G42" s="36">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I42" s="52"/>
-      <c r="J42" s="53"/>
-      <c r="K42" s="51"/>
-      <c r="L42" s="51"/>
-      <c r="M42" s="51"/>
+        <f t="shared" ref="G42:G45" si="4">DAYS360(E42,F42)</f>
+        <v>7</v>
+      </c>
+      <c r="H42" s="37"/>
+      <c r="I42" s="80"/>
+      <c r="J42" s="81"/>
+      <c r="K42" s="82"/>
+      <c r="L42" s="82"/>
+      <c r="M42" s="82"/>
       <c r="N42" s="42"/>
       <c r="O42" s="42"/>
       <c r="P42" s="42"/>
@@ -4878,23 +5338,29 @@
     </row>
     <row r="43" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="32"/>
-      <c r="B43" s="33">
-        <v>4.3</v>
-      </c>
-      <c r="C43" s="45"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
+      <c r="B43" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="89" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" s="35">
+        <v>45217</v>
+      </c>
+      <c r="F43" s="35">
+        <v>45231</v>
+      </c>
       <c r="G43" s="36">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H43" s="37"/>
-      <c r="I43" s="52"/>
-      <c r="J43" s="53"/>
-      <c r="K43" s="51"/>
-      <c r="L43" s="51"/>
-      <c r="M43" s="51"/>
+        <v>14</v>
+      </c>
+      <c r="I43" s="80"/>
+      <c r="J43" s="81"/>
+      <c r="K43" s="82"/>
+      <c r="L43" s="82"/>
+      <c r="M43" s="82"/>
       <c r="N43" s="42"/>
       <c r="O43" s="42"/>
       <c r="P43" s="42"/>
@@ -4963,22 +5429,31 @@
     </row>
     <row r="44" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="32"/>
-      <c r="B44" s="33" t="s">
+      <c r="B44" s="33">
+        <v>4.3</v>
+      </c>
+      <c r="C44" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="45"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
+      <c r="E44" s="35">
+        <v>45231</v>
+      </c>
+      <c r="F44" s="35">
+        <v>45245</v>
+      </c>
       <c r="G44" s="36">
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>14</v>
       </c>
       <c r="H44" s="37"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="53"/>
-      <c r="K44" s="51"/>
-      <c r="L44" s="51"/>
-      <c r="M44" s="51"/>
+      <c r="I44" s="80"/>
+      <c r="J44" s="81"/>
+      <c r="K44" s="82"/>
+      <c r="L44" s="82"/>
+      <c r="M44" s="82"/>
       <c r="N44" s="42"/>
       <c r="O44" s="42"/>
       <c r="P44" s="42"/>
@@ -5045,6 +5520,822 @@
       <c r="BY44" s="38"/>
       <c r="BZ44" s="38"/>
     </row>
+    <row r="45" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="32"/>
+      <c r="B45" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45" s="89" t="s">
+        <v>53</v>
+      </c>
+      <c r="E45" s="35">
+        <v>45245</v>
+      </c>
+      <c r="F45" s="35">
+        <v>45259</v>
+      </c>
+      <c r="G45" s="36">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="H45" s="37"/>
+      <c r="I45" s="80"/>
+      <c r="J45" s="81"/>
+      <c r="K45" s="82"/>
+      <c r="L45" s="82"/>
+      <c r="M45" s="82"/>
+      <c r="N45" s="42"/>
+      <c r="O45" s="42"/>
+      <c r="P45" s="42"/>
+      <c r="Q45" s="42"/>
+      <c r="R45" s="42"/>
+      <c r="S45" s="38"/>
+      <c r="T45" s="38"/>
+      <c r="U45" s="38"/>
+      <c r="V45" s="38"/>
+      <c r="W45" s="38"/>
+      <c r="X45" s="38"/>
+      <c r="Y45" s="38"/>
+      <c r="Z45" s="38"/>
+      <c r="AA45" s="38"/>
+      <c r="AB45" s="38"/>
+      <c r="AC45" s="39"/>
+      <c r="AD45" s="39"/>
+      <c r="AE45" s="39"/>
+      <c r="AF45" s="39"/>
+      <c r="AG45" s="39"/>
+      <c r="AH45" s="38"/>
+      <c r="AI45" s="38"/>
+      <c r="AJ45" s="38"/>
+      <c r="AK45" s="38"/>
+      <c r="AL45" s="38"/>
+      <c r="AM45" s="38"/>
+      <c r="AN45" s="38"/>
+      <c r="AO45" s="38"/>
+      <c r="AP45" s="38"/>
+      <c r="AQ45" s="38"/>
+      <c r="AR45" s="40"/>
+      <c r="AS45" s="40"/>
+      <c r="AT45" s="40"/>
+      <c r="AU45" s="40"/>
+      <c r="AV45" s="40"/>
+      <c r="AW45" s="38"/>
+      <c r="AX45" s="38"/>
+      <c r="AY45" s="38"/>
+      <c r="AZ45" s="38"/>
+      <c r="BA45" s="38"/>
+      <c r="BB45" s="38"/>
+      <c r="BC45" s="38"/>
+      <c r="BD45" s="38"/>
+      <c r="BE45" s="38"/>
+      <c r="BF45" s="38"/>
+      <c r="BG45" s="41"/>
+      <c r="BH45" s="41"/>
+      <c r="BI45" s="41"/>
+      <c r="BJ45" s="41"/>
+      <c r="BK45" s="41"/>
+      <c r="BL45" s="38"/>
+      <c r="BM45" s="38"/>
+      <c r="BN45" s="38"/>
+      <c r="BO45" s="38"/>
+      <c r="BP45" s="38"/>
+      <c r="BQ45" s="38"/>
+      <c r="BR45" s="38"/>
+      <c r="BS45" s="38"/>
+      <c r="BT45" s="38"/>
+      <c r="BU45" s="38"/>
+      <c r="BV45" s="38"/>
+      <c r="BW45" s="38"/>
+      <c r="BX45" s="38"/>
+      <c r="BY45" s="38"/>
+      <c r="BZ45" s="38"/>
+    </row>
+    <row r="46" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="32"/>
+      <c r="B46" s="33">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C46" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="89" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="35">
+        <v>45259</v>
+      </c>
+      <c r="F46" s="35">
+        <v>45273</v>
+      </c>
+      <c r="G46" s="36">
+        <v>14</v>
+      </c>
+      <c r="H46" s="37"/>
+      <c r="I46" s="80"/>
+      <c r="J46" s="81"/>
+      <c r="K46" s="82"/>
+      <c r="L46" s="82"/>
+      <c r="M46" s="82"/>
+      <c r="N46" s="42"/>
+      <c r="O46" s="42"/>
+      <c r="P46" s="42"/>
+      <c r="Q46" s="42"/>
+      <c r="R46" s="42"/>
+      <c r="S46" s="38"/>
+      <c r="T46" s="38"/>
+      <c r="U46" s="38"/>
+      <c r="V46" s="38"/>
+      <c r="W46" s="38"/>
+      <c r="X46" s="38"/>
+      <c r="Y46" s="38"/>
+      <c r="Z46" s="38"/>
+      <c r="AA46" s="38"/>
+      <c r="AB46" s="38"/>
+      <c r="AC46" s="39"/>
+      <c r="AD46" s="39"/>
+      <c r="AE46" s="39"/>
+      <c r="AF46" s="39"/>
+      <c r="AG46" s="39"/>
+      <c r="AH46" s="38"/>
+      <c r="AI46" s="38"/>
+      <c r="AJ46" s="38"/>
+      <c r="AK46" s="38"/>
+      <c r="AL46" s="38"/>
+      <c r="AM46" s="38"/>
+      <c r="AN46" s="38"/>
+      <c r="AO46" s="38"/>
+      <c r="AP46" s="38"/>
+      <c r="AQ46" s="38"/>
+      <c r="AR46" s="40"/>
+      <c r="AS46" s="40"/>
+      <c r="AT46" s="40"/>
+      <c r="AU46" s="40"/>
+      <c r="AV46" s="40"/>
+      <c r="AW46" s="38"/>
+      <c r="AX46" s="38"/>
+      <c r="AY46" s="38"/>
+      <c r="AZ46" s="38"/>
+      <c r="BA46" s="38"/>
+      <c r="BB46" s="38"/>
+      <c r="BC46" s="38"/>
+      <c r="BD46" s="38"/>
+      <c r="BE46" s="38"/>
+      <c r="BF46" s="38"/>
+      <c r="BG46" s="41"/>
+      <c r="BH46" s="41"/>
+      <c r="BI46" s="41"/>
+      <c r="BJ46" s="41"/>
+      <c r="BK46" s="41"/>
+      <c r="BL46" s="38"/>
+      <c r="BM46" s="38"/>
+      <c r="BN46" s="38"/>
+      <c r="BO46" s="38"/>
+      <c r="BP46" s="38"/>
+      <c r="BQ46" s="38"/>
+      <c r="BR46" s="38"/>
+      <c r="BS46" s="38"/>
+      <c r="BT46" s="38"/>
+      <c r="BU46" s="38"/>
+      <c r="BV46" s="38"/>
+      <c r="BW46" s="38"/>
+      <c r="BX46" s="38"/>
+      <c r="BY46" s="38"/>
+      <c r="BZ46" s="38"/>
+    </row>
+    <row r="47" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="26">
+        <v>5</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="53"/>
+      <c r="K47" s="54"/>
+      <c r="L47" s="54"/>
+      <c r="M47" s="52"/>
+      <c r="N47" s="29"/>
+      <c r="O47" s="29"/>
+      <c r="P47" s="29"/>
+      <c r="Q47" s="29"/>
+      <c r="R47" s="29"/>
+      <c r="S47" s="29"/>
+      <c r="T47" s="29"/>
+      <c r="U47" s="29"/>
+      <c r="V47" s="29"/>
+      <c r="W47" s="29"/>
+      <c r="X47" s="29"/>
+      <c r="Y47" s="29"/>
+      <c r="Z47" s="29"/>
+      <c r="AA47" s="29"/>
+      <c r="AB47" s="29"/>
+      <c r="AC47" s="29"/>
+      <c r="AD47" s="29"/>
+      <c r="AE47" s="29"/>
+      <c r="AF47" s="29"/>
+      <c r="AG47" s="29"/>
+      <c r="AH47" s="29"/>
+      <c r="AI47" s="29"/>
+      <c r="AJ47" s="29"/>
+      <c r="AK47" s="29"/>
+      <c r="AL47" s="29"/>
+      <c r="AM47" s="29"/>
+      <c r="AN47" s="29"/>
+      <c r="AO47" s="29"/>
+      <c r="AP47" s="29"/>
+      <c r="AQ47" s="29"/>
+      <c r="AR47" s="29"/>
+      <c r="AS47" s="29"/>
+      <c r="AT47" s="29"/>
+      <c r="AU47" s="29"/>
+      <c r="AV47" s="29"/>
+      <c r="AW47" s="29"/>
+      <c r="AX47" s="29"/>
+      <c r="AY47" s="29"/>
+      <c r="AZ47" s="29"/>
+      <c r="BA47" s="29"/>
+      <c r="BB47" s="29"/>
+      <c r="BC47" s="29"/>
+      <c r="BD47" s="29"/>
+      <c r="BE47" s="29"/>
+      <c r="BF47" s="29"/>
+      <c r="BG47" s="29"/>
+      <c r="BH47" s="29"/>
+      <c r="BI47" s="29"/>
+      <c r="BJ47" s="29"/>
+      <c r="BK47" s="29"/>
+      <c r="BL47" s="29"/>
+      <c r="BM47" s="29"/>
+      <c r="BN47" s="29"/>
+      <c r="BO47" s="29"/>
+      <c r="BP47" s="29"/>
+      <c r="BQ47" s="29"/>
+      <c r="BR47" s="29"/>
+      <c r="BS47" s="29"/>
+      <c r="BT47" s="29"/>
+      <c r="BU47" s="29"/>
+      <c r="BV47" s="29"/>
+      <c r="BW47" s="29"/>
+      <c r="BX47" s="29"/>
+      <c r="BY47" s="29"/>
+      <c r="BZ47" s="29"/>
+    </row>
+    <row r="48" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="33">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C48" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" s="35">
+        <v>45203</v>
+      </c>
+      <c r="F48" s="35">
+        <v>45210</v>
+      </c>
+      <c r="G48" s="36">
+        <f>DAYS360(E48,F48)</f>
+        <v>7</v>
+      </c>
+      <c r="H48" s="37"/>
+      <c r="I48" s="80"/>
+      <c r="J48" s="81"/>
+      <c r="K48" s="82"/>
+      <c r="L48" s="82"/>
+      <c r="M48" s="82"/>
+      <c r="N48" s="42"/>
+      <c r="O48" s="42"/>
+      <c r="P48" s="42"/>
+      <c r="Q48" s="42"/>
+      <c r="R48" s="42"/>
+      <c r="S48" s="38"/>
+      <c r="T48" s="38"/>
+      <c r="U48" s="38"/>
+      <c r="V48" s="38"/>
+      <c r="W48" s="38"/>
+      <c r="X48" s="38"/>
+      <c r="Y48" s="38"/>
+      <c r="Z48" s="38"/>
+      <c r="AA48" s="38"/>
+      <c r="AB48" s="38"/>
+      <c r="AC48" s="39"/>
+      <c r="AD48" s="39"/>
+      <c r="AE48" s="39"/>
+      <c r="AF48" s="39"/>
+      <c r="AG48" s="39"/>
+      <c r="AH48" s="38"/>
+      <c r="AI48" s="38"/>
+      <c r="AJ48" s="38"/>
+      <c r="AK48" s="38"/>
+      <c r="AL48" s="38"/>
+      <c r="AM48" s="38"/>
+      <c r="AN48" s="38"/>
+      <c r="AO48" s="38"/>
+      <c r="AP48" s="38"/>
+      <c r="AQ48" s="38"/>
+      <c r="AR48" s="40"/>
+      <c r="AS48" s="40"/>
+      <c r="AT48" s="40"/>
+      <c r="AU48" s="40"/>
+      <c r="AV48" s="40"/>
+      <c r="AW48" s="38"/>
+      <c r="AX48" s="38"/>
+      <c r="AY48" s="38"/>
+      <c r="AZ48" s="38"/>
+      <c r="BA48" s="38"/>
+      <c r="BB48" s="38"/>
+      <c r="BC48" s="38"/>
+      <c r="BD48" s="38"/>
+      <c r="BE48" s="38"/>
+      <c r="BF48" s="38"/>
+      <c r="BG48" s="41"/>
+      <c r="BH48" s="41"/>
+      <c r="BI48" s="41"/>
+      <c r="BJ48" s="41"/>
+      <c r="BK48" s="41"/>
+      <c r="BL48" s="38"/>
+      <c r="BM48" s="38"/>
+      <c r="BN48" s="38"/>
+      <c r="BO48" s="38"/>
+      <c r="BP48" s="38"/>
+      <c r="BQ48" s="38"/>
+      <c r="BR48" s="38"/>
+      <c r="BS48" s="38"/>
+      <c r="BT48" s="38"/>
+      <c r="BU48" s="38"/>
+      <c r="BV48" s="38"/>
+      <c r="BW48" s="38"/>
+      <c r="BX48" s="38"/>
+      <c r="BY48" s="38"/>
+      <c r="BZ48" s="38"/>
+    </row>
+    <row r="49" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="33">
+        <v>4.2</v>
+      </c>
+      <c r="C49" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="D49" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="E49" s="35">
+        <v>45210</v>
+      </c>
+      <c r="F49" s="35">
+        <v>45217</v>
+      </c>
+      <c r="G49" s="36">
+        <v>7</v>
+      </c>
+      <c r="H49" s="37"/>
+      <c r="I49" s="80"/>
+      <c r="J49" s="81"/>
+      <c r="K49" s="82"/>
+      <c r="L49" s="82"/>
+      <c r="M49" s="82"/>
+      <c r="N49" s="42"/>
+      <c r="O49" s="42"/>
+      <c r="P49" s="42"/>
+      <c r="Q49" s="42"/>
+      <c r="R49" s="42"/>
+      <c r="S49" s="38"/>
+      <c r="T49" s="38"/>
+      <c r="U49" s="38"/>
+      <c r="V49" s="38"/>
+      <c r="W49" s="38"/>
+      <c r="X49" s="38"/>
+      <c r="Y49" s="38"/>
+      <c r="Z49" s="38"/>
+      <c r="AA49" s="38"/>
+      <c r="AB49" s="38"/>
+      <c r="AC49" s="39"/>
+      <c r="AD49" s="39"/>
+      <c r="AE49" s="39"/>
+      <c r="AF49" s="39"/>
+      <c r="AG49" s="39"/>
+      <c r="AH49" s="38"/>
+      <c r="AI49" s="38"/>
+      <c r="AJ49" s="38"/>
+      <c r="AK49" s="38"/>
+      <c r="AL49" s="38"/>
+      <c r="AM49" s="38"/>
+      <c r="AN49" s="38"/>
+      <c r="AO49" s="38"/>
+      <c r="AP49" s="38"/>
+      <c r="AQ49" s="38"/>
+      <c r="AR49" s="40"/>
+      <c r="AS49" s="40"/>
+      <c r="AT49" s="40"/>
+      <c r="AU49" s="40"/>
+      <c r="AV49" s="40"/>
+      <c r="AW49" s="38"/>
+      <c r="AX49" s="38"/>
+      <c r="AY49" s="38"/>
+      <c r="AZ49" s="38"/>
+      <c r="BA49" s="38"/>
+      <c r="BB49" s="38"/>
+      <c r="BC49" s="38"/>
+      <c r="BD49" s="38"/>
+      <c r="BE49" s="38"/>
+      <c r="BF49" s="38"/>
+      <c r="BG49" s="41"/>
+      <c r="BH49" s="41"/>
+      <c r="BI49" s="41"/>
+      <c r="BJ49" s="41"/>
+      <c r="BK49" s="41"/>
+      <c r="BL49" s="38"/>
+      <c r="BM49" s="38"/>
+      <c r="BN49" s="38"/>
+      <c r="BO49" s="38"/>
+      <c r="BP49" s="38"/>
+      <c r="BQ49" s="38"/>
+      <c r="BR49" s="38"/>
+      <c r="BS49" s="38"/>
+      <c r="BT49" s="38"/>
+      <c r="BU49" s="38"/>
+      <c r="BV49" s="38"/>
+      <c r="BW49" s="38"/>
+      <c r="BX49" s="38"/>
+      <c r="BY49" s="38"/>
+      <c r="BZ49" s="38"/>
+    </row>
+    <row r="50" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="E50" s="35">
+        <v>45217</v>
+      </c>
+      <c r="F50" s="35">
+        <v>45231</v>
+      </c>
+      <c r="G50" s="36">
+        <v>14</v>
+      </c>
+      <c r="H50" s="37"/>
+      <c r="I50" s="80"/>
+      <c r="J50" s="81"/>
+      <c r="K50" s="82"/>
+      <c r="L50" s="82"/>
+      <c r="M50" s="82"/>
+      <c r="N50" s="42"/>
+      <c r="O50" s="42"/>
+      <c r="P50" s="42"/>
+      <c r="Q50" s="42"/>
+      <c r="R50" s="42"/>
+      <c r="S50" s="38"/>
+      <c r="T50" s="38"/>
+      <c r="U50" s="38"/>
+      <c r="V50" s="38"/>
+      <c r="W50" s="38"/>
+      <c r="X50" s="38"/>
+      <c r="Y50" s="38"/>
+      <c r="Z50" s="38"/>
+      <c r="AA50" s="38"/>
+      <c r="AB50" s="38"/>
+      <c r="AC50" s="39"/>
+      <c r="AD50" s="39"/>
+      <c r="AE50" s="39"/>
+      <c r="AF50" s="39"/>
+      <c r="AG50" s="39"/>
+      <c r="AH50" s="38"/>
+      <c r="AI50" s="38"/>
+      <c r="AJ50" s="38"/>
+      <c r="AK50" s="38"/>
+      <c r="AL50" s="38"/>
+      <c r="AM50" s="38"/>
+      <c r="AN50" s="38"/>
+      <c r="AO50" s="38"/>
+      <c r="AP50" s="38"/>
+      <c r="AQ50" s="38"/>
+      <c r="AR50" s="40"/>
+      <c r="AS50" s="40"/>
+      <c r="AT50" s="40"/>
+      <c r="AU50" s="40"/>
+      <c r="AV50" s="40"/>
+      <c r="AW50" s="38"/>
+      <c r="AX50" s="38"/>
+      <c r="AY50" s="38"/>
+      <c r="AZ50" s="38"/>
+      <c r="BA50" s="38"/>
+      <c r="BB50" s="38"/>
+      <c r="BC50" s="38"/>
+      <c r="BD50" s="38"/>
+      <c r="BE50" s="38"/>
+      <c r="BF50" s="38"/>
+      <c r="BG50" s="41"/>
+      <c r="BH50" s="41"/>
+      <c r="BI50" s="41"/>
+      <c r="BJ50" s="41"/>
+      <c r="BK50" s="41"/>
+      <c r="BL50" s="38"/>
+      <c r="BM50" s="38"/>
+      <c r="BN50" s="38"/>
+      <c r="BO50" s="38"/>
+      <c r="BP50" s="38"/>
+      <c r="BQ50" s="38"/>
+      <c r="BR50" s="38"/>
+      <c r="BS50" s="38"/>
+      <c r="BT50" s="38"/>
+      <c r="BU50" s="38"/>
+      <c r="BV50" s="38"/>
+      <c r="BW50" s="38"/>
+      <c r="BX50" s="38"/>
+      <c r="BY50" s="38"/>
+      <c r="BZ50" s="38"/>
+    </row>
+    <row r="51" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" s="57" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="E51" s="35">
+        <v>45231</v>
+      </c>
+      <c r="F51" s="35">
+        <v>45245</v>
+      </c>
+      <c r="G51" s="36">
+        <f t="shared" ref="G50:G52" si="5">DAYS360(E51,F51)</f>
+        <v>14</v>
+      </c>
+      <c r="I51" s="80"/>
+      <c r="J51" s="81"/>
+      <c r="K51" s="82"/>
+      <c r="L51" s="82"/>
+      <c r="M51" s="82"/>
+      <c r="N51" s="42"/>
+      <c r="O51" s="42"/>
+      <c r="P51" s="42"/>
+      <c r="Q51" s="42"/>
+      <c r="R51" s="42"/>
+      <c r="S51" s="38"/>
+      <c r="T51" s="38"/>
+      <c r="U51" s="38"/>
+      <c r="V51" s="38"/>
+      <c r="W51" s="38"/>
+      <c r="X51" s="38"/>
+      <c r="Y51" s="38"/>
+      <c r="Z51" s="38"/>
+      <c r="AA51" s="38"/>
+      <c r="AB51" s="38"/>
+      <c r="AC51" s="39"/>
+      <c r="AD51" s="39"/>
+      <c r="AE51" s="39"/>
+      <c r="AF51" s="39"/>
+      <c r="AG51" s="39"/>
+      <c r="AH51" s="38"/>
+      <c r="AI51" s="38"/>
+      <c r="AJ51" s="38"/>
+      <c r="AK51" s="38"/>
+      <c r="AL51" s="38"/>
+      <c r="AM51" s="38"/>
+      <c r="AN51" s="38"/>
+      <c r="AO51" s="38"/>
+      <c r="AP51" s="38"/>
+      <c r="AQ51" s="38"/>
+      <c r="AR51" s="40"/>
+      <c r="AS51" s="40"/>
+      <c r="AT51" s="40"/>
+      <c r="AU51" s="40"/>
+      <c r="AV51" s="40"/>
+      <c r="AW51" s="38"/>
+      <c r="AX51" s="38"/>
+      <c r="AY51" s="38"/>
+      <c r="AZ51" s="38"/>
+      <c r="BA51" s="38"/>
+      <c r="BB51" s="38"/>
+      <c r="BC51" s="38"/>
+      <c r="BD51" s="38"/>
+      <c r="BE51" s="38"/>
+      <c r="BF51" s="38"/>
+      <c r="BG51" s="41"/>
+      <c r="BH51" s="41"/>
+      <c r="BI51" s="41"/>
+      <c r="BJ51" s="41"/>
+      <c r="BK51" s="41"/>
+      <c r="BL51" s="38"/>
+      <c r="BM51" s="38"/>
+      <c r="BN51" s="38"/>
+      <c r="BO51" s="38"/>
+      <c r="BP51" s="38"/>
+      <c r="BQ51" s="38"/>
+      <c r="BR51" s="38"/>
+      <c r="BS51" s="38"/>
+      <c r="BT51" s="38"/>
+      <c r="BU51" s="38"/>
+      <c r="BV51" s="38"/>
+      <c r="BW51" s="38"/>
+      <c r="BX51" s="38"/>
+      <c r="BY51" s="38"/>
+      <c r="BZ51" s="38"/>
+    </row>
+    <row r="52" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="33">
+        <v>4.3</v>
+      </c>
+      <c r="C52" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="D52" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="E52" s="35">
+        <v>45245</v>
+      </c>
+      <c r="F52" s="35">
+        <v>45259</v>
+      </c>
+      <c r="G52" s="36">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="H52" s="37"/>
+      <c r="I52" s="80"/>
+      <c r="J52" s="81"/>
+      <c r="K52" s="82"/>
+      <c r="L52" s="82"/>
+      <c r="M52" s="82"/>
+      <c r="N52" s="42"/>
+      <c r="O52" s="42"/>
+      <c r="P52" s="42"/>
+      <c r="Q52" s="42"/>
+      <c r="R52" s="42"/>
+      <c r="S52" s="38"/>
+      <c r="T52" s="38"/>
+      <c r="U52" s="38"/>
+      <c r="V52" s="38"/>
+      <c r="W52" s="38"/>
+      <c r="X52" s="38"/>
+      <c r="Y52" s="38"/>
+      <c r="Z52" s="38"/>
+      <c r="AA52" s="38"/>
+      <c r="AB52" s="38"/>
+      <c r="AC52" s="39"/>
+      <c r="AD52" s="39"/>
+      <c r="AE52" s="39"/>
+      <c r="AF52" s="39"/>
+      <c r="AG52" s="39"/>
+      <c r="AH52" s="38"/>
+      <c r="AI52" s="38"/>
+      <c r="AJ52" s="38"/>
+      <c r="AK52" s="38"/>
+      <c r="AL52" s="38"/>
+      <c r="AM52" s="38"/>
+      <c r="AN52" s="38"/>
+      <c r="AO52" s="38"/>
+      <c r="AP52" s="38"/>
+      <c r="AQ52" s="38"/>
+      <c r="AR52" s="40"/>
+      <c r="AS52" s="40"/>
+      <c r="AT52" s="40"/>
+      <c r="AU52" s="40"/>
+      <c r="AV52" s="40"/>
+      <c r="AW52" s="38"/>
+      <c r="AX52" s="38"/>
+      <c r="AY52" s="38"/>
+      <c r="AZ52" s="38"/>
+      <c r="BA52" s="38"/>
+      <c r="BB52" s="38"/>
+      <c r="BC52" s="38"/>
+      <c r="BD52" s="38"/>
+      <c r="BE52" s="38"/>
+      <c r="BF52" s="38"/>
+      <c r="BG52" s="41"/>
+      <c r="BH52" s="41"/>
+      <c r="BI52" s="41"/>
+      <c r="BJ52" s="41"/>
+      <c r="BK52" s="41"/>
+      <c r="BL52" s="38"/>
+      <c r="BM52" s="38"/>
+      <c r="BN52" s="38"/>
+      <c r="BO52" s="38"/>
+      <c r="BP52" s="38"/>
+      <c r="BQ52" s="38"/>
+      <c r="BR52" s="38"/>
+      <c r="BS52" s="38"/>
+      <c r="BT52" s="38"/>
+      <c r="BU52" s="38"/>
+      <c r="BV52" s="38"/>
+      <c r="BW52" s="38"/>
+      <c r="BX52" s="38"/>
+      <c r="BY52" s="38"/>
+      <c r="BZ52" s="38"/>
+    </row>
+    <row r="53" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="D53" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="E53" s="35">
+        <v>45259</v>
+      </c>
+      <c r="F53" s="35">
+        <v>45273</v>
+      </c>
+      <c r="G53" s="36">
+        <v>14</v>
+      </c>
+      <c r="H53" s="37"/>
+      <c r="I53" s="80"/>
+      <c r="J53" s="81"/>
+      <c r="K53" s="82"/>
+      <c r="L53" s="82"/>
+      <c r="M53" s="82"/>
+      <c r="N53" s="42"/>
+      <c r="O53" s="42"/>
+      <c r="P53" s="42"/>
+      <c r="Q53" s="42"/>
+      <c r="R53" s="42"/>
+      <c r="S53" s="38"/>
+      <c r="T53" s="38"/>
+      <c r="U53" s="38"/>
+      <c r="V53" s="38"/>
+      <c r="W53" s="38"/>
+      <c r="X53" s="38"/>
+      <c r="Y53" s="38"/>
+      <c r="Z53" s="38"/>
+      <c r="AA53" s="38"/>
+      <c r="AB53" s="38"/>
+      <c r="AC53" s="39"/>
+      <c r="AD53" s="39"/>
+      <c r="AE53" s="39"/>
+      <c r="AF53" s="39"/>
+      <c r="AG53" s="39"/>
+      <c r="AH53" s="38"/>
+      <c r="AI53" s="38"/>
+      <c r="AJ53" s="38"/>
+      <c r="AK53" s="38"/>
+      <c r="AL53" s="38"/>
+      <c r="AM53" s="38"/>
+      <c r="AN53" s="38"/>
+      <c r="AO53" s="38"/>
+      <c r="AP53" s="38"/>
+      <c r="AQ53" s="38"/>
+      <c r="AR53" s="40"/>
+      <c r="AS53" s="40"/>
+      <c r="AT53" s="40"/>
+      <c r="AU53" s="40"/>
+      <c r="AV53" s="40"/>
+      <c r="AW53" s="38"/>
+      <c r="AX53" s="38"/>
+      <c r="AY53" s="38"/>
+      <c r="AZ53" s="38"/>
+      <c r="BA53" s="38"/>
+      <c r="BB53" s="38"/>
+      <c r="BC53" s="38"/>
+      <c r="BD53" s="38"/>
+      <c r="BE53" s="38"/>
+      <c r="BF53" s="38"/>
+      <c r="BG53" s="41"/>
+      <c r="BH53" s="41"/>
+      <c r="BI53" s="41"/>
+      <c r="BJ53" s="41"/>
+      <c r="BK53" s="41"/>
+      <c r="BL53" s="38"/>
+      <c r="BM53" s="38"/>
+      <c r="BN53" s="38"/>
+      <c r="BO53" s="38"/>
+      <c r="BP53" s="38"/>
+      <c r="BQ53" s="38"/>
+      <c r="BR53" s="38"/>
+      <c r="BS53" s="38"/>
+      <c r="BT53" s="38"/>
+      <c r="BU53" s="38"/>
+      <c r="BV53" s="38"/>
+      <c r="BW53" s="38"/>
+      <c r="BX53" s="38"/>
+      <c r="BY53" s="38"/>
+      <c r="BZ53" s="38"/>
+    </row>
   </sheetData>
   <mergeCells count="36">
     <mergeCell ref="E8:E9"/>
@@ -5084,7 +6375,7 @@
     <mergeCell ref="BV9:BZ9"/>
     <mergeCell ref="S9:W9"/>
   </mergeCells>
-  <conditionalFormatting sqref="H11:H17 H19:H44">
+  <conditionalFormatting sqref="H11:H17 H19:H53">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>